<commit_message>
Oracle-DinhSang: four week rebuild practice
</commit_message>
<xml_diff>
--- a/ThirdWeek/Practice/Practice.xlsx
+++ b/ThirdWeek/Practice/Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sangnd\Desktop\SSGTraining_Oracle\ThirdWeek\Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2040B3E4-F70C-416B-BB8D-343F3899E4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FCC347-8335-4CC2-BDB8-4882A2FEAE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{04339533-6319-4BDC-AC42-7B00236AED5D}"/>
   </bookViews>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554B0E0D-7F36-495B-AF44-FF541208BFF5}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>